<commit_message>
aggiunto misure resistenza amperometro
</commit_message>
<xml_diff>
--- a/circuiti 20240307/20240307circuiti.xlsx
+++ b/circuiti 20240307/20240307circuiti.xlsx
@@ -3,17 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="voltmetro" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="amperometro" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>R(MOHM)</t>
   </si>
@@ -22,6 +23,12 @@
   </si>
   <si>
     <t>V</t>
+  </si>
+  <si>
+    <t>R(OHM)</t>
+  </si>
+  <si>
+    <t>I(A)</t>
   </si>
 </sst>
 </file>
@@ -56,8 +63,9 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,4 +759,142 @@
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2.1099999999999999</v>
+      </c>
+      <c r="C2">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="C3">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2.6000000000000001</v>
+      </c>
+      <c r="C4">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2.6400000000000001</v>
+      </c>
+      <c r="C5">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2.6600000000000001</v>
+      </c>
+      <c r="C6">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2.6800000000000002</v>
+      </c>
+      <c r="C7">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2.7000000000000002</v>
+      </c>
+      <c r="C8">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2.7000000000000002</v>
+      </c>
+      <c r="C9">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2.71</v>
+      </c>
+      <c r="C10">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2.7200000000000002</v>
+      </c>
+      <c r="C11">
+        <v>248</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>